<commit_message>
Changed RobotsFactory.xlsx headings background
</commit_message>
<xml_diff>
--- a/Reports/RobotsFactory.xlsx
+++ b/Reports/RobotsFactory.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bressan\Documents\GitHub\Databases-Teamwork-2014\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivaylo\Dropbox\Ivo\IT\Telerik Academy\Telerik Academy 2013 (Database, Teamwork)\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="24000" windowHeight="9735" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="24000" windowHeight="9735" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -374,12 +374,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -422,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -431,16 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -454,6 +451,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,529 +759,529 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="9" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>95</v>
       </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="5">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
         <v>2014</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>450000</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>80</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>2</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="5">
+      <c r="G4" s="5"/>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
         <v>2013</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>250000</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>50</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>3</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="G5" s="5"/>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
         <v>2010</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>221000</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>75</v>
       </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="5">
-        <v>1</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
         <v>2008</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>365000</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>0.05</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>5</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5">
+      <c r="G7" s="5"/>
+      <c r="H7" s="4">
         <v>8</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>2001</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>120</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>0.6</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>4</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="5">
+      <c r="G8" s="5"/>
+      <c r="H8" s="4">
         <v>3</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>2004</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>631.25</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>0.08</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>7</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="5">
+      <c r="G9" s="5"/>
+      <c r="H9" s="4">
         <v>4</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>2006</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>234.21</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>0.05</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>12</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="5">
+      <c r="G10" s="5"/>
+      <c r="H10" s="4">
         <v>7</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>2004</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>85.2</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>65</v>
       </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>2</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>2007</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="4">
         <v>402350</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>2.4</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>6</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
         <v>2007</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <v>123</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>1.18</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>8</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="5">
+      <c r="G13" s="5"/>
+      <c r="H13" s="4">
         <v>5</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <v>2013</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="4">
         <v>999</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>1.3</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>8</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="5">
+      <c r="G14" s="5"/>
+      <c r="H14" s="4">
         <v>5</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="4">
         <v>2011</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="4">
         <v>1400</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>13</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>700</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>10</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="5">
+      <c r="G15" s="5"/>
+      <c r="H15" s="4">
         <v>6</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="4">
         <v>2013</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="4">
         <v>80000</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>2</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>9</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="5">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5">
+      <c r="H16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
         <v>2009</v>
       </c>
-      <c r="J16" s="5">
+      <c r="J16" s="4">
         <v>15000</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>15</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>40</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>11</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <v>7</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="4">
         <v>2008</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="4">
         <v>80.23</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>3</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>8</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="5">
+      <c r="G18" s="5"/>
+      <c r="H18" s="4">
         <v>9</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <v>2010</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="4">
         <v>250.3</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>1.2</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>3</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="5">
+      <c r="G19" s="5"/>
+      <c r="H19" s="4">
         <v>11</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <v>2014</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="4">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>18</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>3.4</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>8</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="5">
+      <c r="G20" s="5"/>
+      <c r="H20" s="4">
         <v>10</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="4">
         <v>2011</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="4">
         <v>27500</v>
       </c>
     </row>
@@ -1293,7 +1296,7 @@
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,106 +1308,106 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1418,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D4:D13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,134 +1435,134 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>11</v>
       </c>
     </row>
@@ -1574,7 +1577,7 @@
   <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,134 +1589,134 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>10</v>
       </c>
     </row>
@@ -1728,7 +1731,7 @@
   <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,123 +1744,123 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1871,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,66 +1887,66 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <v>6</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
+      <c r="B9" s="7">
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Robots Factory Excel File Updated
</commit_message>
<xml_diff>
--- a/Reports/RobotsFactory.xlsx
+++ b/Reports/RobotsFactory.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivaylo\Dropbox\Ivo\IT\Telerik Academy\Telerik Academy 2013 (Database, Teamwork)\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bressan\Documents\GitHub\Databases-Teamwork-2014\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="24000" windowHeight="9735" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Manufacturers" sheetId="3" r:id="rId3"/>
     <sheet name="Addresses" sheetId="4" r:id="rId4"/>
     <sheet name="Cities" sheetId="5" r:id="rId5"/>
-    <sheet name="Contries" sheetId="6" r:id="rId6"/>
+    <sheet name="Countries" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,9 +31,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
   <si>
-    <t>ProductID</t>
-  </si>
-  <si>
     <t>ProductName</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>24 Rusevelt Ave, Pensacola, Florida</t>
+  </si>
+  <si>
+    <t>ProductId</t>
   </si>
 </sst>
 </file>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,31 +760,31 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="D2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -792,10 +792,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="4">
         <v>95</v>
@@ -804,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="4">
         <v>1</v>
@@ -821,10 +821,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4">
         <v>80</v>
@@ -848,10 +848,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="4">
         <v>50</v>
@@ -875,10 +875,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="4">
         <v>75</v>
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>
@@ -904,10 +904,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="4">
         <v>0.05</v>
@@ -931,10 +931,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="4">
         <v>0.6</v>
@@ -958,10 +958,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" s="4">
         <v>0.08</v>
@@ -985,10 +985,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="4">
         <v>0.05</v>
@@ -1012,10 +1012,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="4">
         <v>65</v>
@@ -1024,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="4">
         <v>2</v>
@@ -1041,10 +1041,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="4">
         <v>2.4</v>
@@ -1053,7 +1053,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H12" s="4">
         <v>1</v>
@@ -1070,10 +1070,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="4">
         <v>1.18</v>
@@ -1097,10 +1097,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E14" s="4">
         <v>1.3</v>
@@ -1124,10 +1124,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="4">
         <v>700</v>
@@ -1151,10 +1151,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" s="4">
         <v>2</v>
@@ -1163,7 +1163,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" s="4">
         <v>1</v>
@@ -1180,10 +1180,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="4">
         <v>40</v>
@@ -1192,7 +1192,7 @@
         <v>11</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H17" s="4">
         <v>7</v>
@@ -1209,10 +1209,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="4">
         <v>3</v>
@@ -1236,10 +1236,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E19" s="4">
         <v>1.2</v>
@@ -1263,10 +1263,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" s="4">
         <v>3.4</v>
@@ -1309,10 +1309,10 @@
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1320,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1328,7 +1328,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1336,7 +1336,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1344,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1352,7 +1352,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1360,7 +1360,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1368,7 +1368,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1376,7 +1376,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1384,7 +1384,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1392,7 +1392,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1400,7 +1400,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1408,7 +1408,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1436,13 +1436,13 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1461,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
@@ -1472,7 +1472,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="7">
         <v>3</v>
@@ -1483,7 +1483,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
@@ -1494,7 +1494,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="7">
         <v>5</v>
@@ -1505,7 +1505,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="7">
         <v>6</v>
@@ -1516,7 +1516,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="7">
         <v>7</v>
@@ -1527,7 +1527,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="7">
         <v>8</v>
@@ -1538,7 +1538,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7">
         <v>9</v>
@@ -1549,7 +1549,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="7">
         <v>10</v>
@@ -1560,7 +1560,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="7">
         <v>11</v>
@@ -1590,13 +1590,13 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1604,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1615,7 +1615,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -1626,7 +1626,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -1637,7 +1637,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="4">
         <v>4</v>
@@ -1648,7 +1648,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="4">
         <v>5</v>
@@ -1659,7 +1659,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -1670,7 +1670,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="4">
         <v>6</v>
@@ -1681,7 +1681,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="4">
         <v>7</v>
@@ -1692,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11" s="4">
         <v>8</v>
@@ -1703,7 +1703,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" s="4">
         <v>9</v>
@@ -1714,7 +1714,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13" s="4">
         <v>10</v>
@@ -1745,13 +1745,13 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1759,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1770,7 +1770,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="4">
         <v>6</v>
@@ -1781,7 +1781,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1792,7 +1792,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -1803,7 +1803,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="4">
         <v>7</v>
@@ -1814,7 +1814,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="4">
         <v>3</v>
@@ -1825,7 +1825,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1836,7 +1836,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -1847,7 +1847,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
@@ -1858,7 +1858,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -1874,7 +1874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1888,10 +1888,10 @@
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1899,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1907,7 +1907,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1915,7 +1915,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1923,7 +1923,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1931,7 +1931,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1939,7 +1939,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1947,7 +1947,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CentralDatabaseSeeder Template Method added MongoDbSeeder class added -> Read data from cloud database and seed data in MSSQL Product class property Weight type changed
</commit_message>
<xml_diff>
--- a/Reports/RobotsFactory.xlsx
+++ b/Reports/RobotsFactory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -29,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="107">
-  <si>
-    <t>ProductName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>ManufacturerID</t>
   </si>
@@ -740,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,31 +757,31 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="I2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -792,10 +789,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="4">
         <v>95</v>
@@ -804,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" s="4">
         <v>1</v>
@@ -821,10 +818,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4">
         <v>80</v>
@@ -848,10 +845,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="4">
         <v>50</v>
@@ -875,10 +872,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="4">
         <v>75</v>
@@ -887,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>
@@ -904,10 +901,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="4">
         <v>0.05</v>
@@ -931,10 +928,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4">
         <v>0.6</v>
@@ -958,10 +955,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="4">
         <v>0.08</v>
@@ -985,10 +982,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="4">
         <v>0.05</v>
@@ -1012,10 +1009,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="4">
         <v>65</v>
@@ -1024,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="4">
         <v>2</v>
@@ -1041,10 +1038,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="4">
         <v>2.4</v>
@@ -1053,7 +1050,7 @@
         <v>6</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="4">
         <v>1</v>
@@ -1070,10 +1067,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="4">
         <v>1.18</v>
@@ -1097,10 +1094,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="4">
         <v>1.3</v>
@@ -1124,10 +1121,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="4">
         <v>700</v>
@@ -1151,10 +1148,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" s="4">
         <v>2</v>
@@ -1163,7 +1160,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H16" s="4">
         <v>1</v>
@@ -1180,10 +1177,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="4">
         <v>40</v>
@@ -1192,7 +1189,7 @@
         <v>11</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H17" s="4">
         <v>7</v>
@@ -1209,10 +1206,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" s="4">
         <v>3</v>
@@ -1236,10 +1233,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="4">
         <v>1.2</v>
@@ -1263,10 +1260,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="4">
         <v>3.4</v>
@@ -1309,10 +1306,10 @@
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1320,7 +1317,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1328,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1336,7 +1333,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1344,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1352,7 +1349,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1360,7 +1357,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1368,7 +1365,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1376,7 +1373,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1384,7 +1381,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1392,7 +1389,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1400,7 +1397,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1408,7 +1405,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1436,13 +1433,13 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1450,7 +1447,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1461,7 +1458,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
@@ -1472,7 +1469,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="7">
         <v>3</v>
@@ -1483,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
@@ -1494,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="7">
         <v>5</v>
@@ -1505,7 +1502,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="7">
         <v>6</v>
@@ -1516,7 +1513,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="7">
         <v>7</v>
@@ -1527,7 +1524,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="7">
         <v>8</v>
@@ -1538,7 +1535,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="7">
         <v>9</v>
@@ -1549,7 +1546,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="7">
         <v>10</v>
@@ -1560,7 +1557,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="7">
         <v>11</v>
@@ -1590,13 +1587,13 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1604,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1615,7 +1612,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -1626,7 +1623,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
@@ -1637,7 +1634,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="4">
         <v>4</v>
@@ -1648,7 +1645,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="4">
         <v>5</v>
@@ -1659,7 +1656,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
@@ -1670,7 +1667,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="4">
         <v>6</v>
@@ -1681,7 +1678,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="4">
         <v>7</v>
@@ -1692,7 +1689,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" s="4">
         <v>8</v>
@@ -1703,7 +1700,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12" s="4">
         <v>9</v>
@@ -1714,7 +1711,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="4">
         <v>10</v>
@@ -1745,13 +1742,13 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1759,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -1770,7 +1767,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="4">
         <v>6</v>
@@ -1781,7 +1778,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1792,7 +1789,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -1803,7 +1800,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="4">
         <v>7</v>
@@ -1814,7 +1811,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="4">
         <v>3</v>
@@ -1825,7 +1822,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1836,7 +1833,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -1847,7 +1844,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="4">
         <v>4</v>
@@ -1858,7 +1855,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -1888,10 +1885,10 @@
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1899,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1907,7 +1904,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1915,7 +1912,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1923,7 +1920,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1931,7 +1928,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1939,7 +1936,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1947,7 +1944,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>